<commit_message>
Load Balancer WebServer and StorageServer
</commit_message>
<xml_diff>
--- a/docs/LVTN_DeTaiChiaSeVideo_Planing 26.11 - 02.12.xlsx
+++ b/docs/LVTN_DeTaiChiaSeVideo_Planing 26.11 - 02.12.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="86">
   <si>
     <t>Thời gian thực hiện</t>
   </si>
@@ -206,9 +206,6 @@
     <t>Coding Backend</t>
   </si>
   <si>
-    <t>Hiễn thị lên web từ database</t>
-  </si>
-  <si>
     <t>29/11</t>
   </si>
   <si>
@@ -279,6 +276,13 @@
   </si>
   <si>
     <t xml:space="preserve"> - hỗ trợ Voice Control cho các function can bản: next, previos, mute, delay, resume, replay…</t>
+  </si>
+  <si>
+    <t>chưa test trên 2 máy riêng biệt
+đã test trên 2 server tomcat trên cùng 1 laptop</t>
+  </si>
+  <si>
+    <t>Hiễn thị lên web từ database kèm Recommend</t>
   </si>
 </sst>
 </file>
@@ -415,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -481,32 +485,35 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -815,8 +822,8 @@
   <dimension ref="B1:O59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
+      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B46" sqref="B46:H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,26 +831,27 @@
     <col min="2" max="2" width="36.5703125" customWidth="1"/>
     <col min="3" max="3" width="20.140625" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" style="18" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" customWidth="1"/>
-    <col min="6" max="6" width="34.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="41.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
     <col min="8" max="8" width="21.42578125" customWidth="1"/>
     <col min="9" max="9" width="51.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B1" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
+      <c r="B1" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
     </row>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>18</v>
@@ -872,15 +880,15 @@
       </c>
     </row>
     <row r="3" spans="2:15" ht="21" x14ac:dyDescent="0.25">
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="34"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="38"/>
       <c r="N3" s="6" t="s">
         <v>19</v>
       </c>
@@ -1057,15 +1065,15 @@
       </c>
     </row>
     <row r="14" spans="2:15" ht="21" x14ac:dyDescent="0.25">
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
@@ -1174,15 +1182,15 @@
       </c>
     </row>
     <row r="23" spans="2:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
     </row>
     <row r="24" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B24" s="11" t="s">
@@ -1262,7 +1270,7 @@
         <v>41</v>
       </c>
       <c r="E28" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="6">
@@ -1273,15 +1281,15 @@
       </c>
     </row>
     <row r="29" spans="2:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="B29" s="35" t="s">
+      <c r="B29" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="34"/>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
@@ -1347,26 +1355,26 @@
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="C33" s="39"/>
-      <c r="D33" s="39"/>
-      <c r="E33" s="39"/>
-      <c r="F33" s="39"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="39"/>
+      <c r="B33" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
     </row>
     <row r="34" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B34" s="37" t="s">
+      <c r="B34" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="C34" s="37"/>
-      <c r="D34" s="37"/>
-      <c r="E34" s="37"/>
-      <c r="F34" s="37"/>
-      <c r="G34" s="37"/>
-      <c r="H34" s="37"/>
+      <c r="C34" s="39"/>
+      <c r="D34" s="39"/>
+      <c r="E34" s="39"/>
+      <c r="F34" s="39"/>
+      <c r="G34" s="39"/>
+      <c r="H34" s="39"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
@@ -1379,10 +1387,10 @@
         <v>41</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F35" t="s">
         <v>60</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="G35" s="2"/>
       <c r="H35" s="2" t="s">
@@ -1400,10 +1408,10 @@
         <v>41</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F36" t="s">
         <v>60</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2" t="s">
@@ -1421,10 +1429,10 @@
         <v>41</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F37" t="s">
         <v>60</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2" t="s">
@@ -1442,10 +1450,10 @@
         <v>41</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F38" t="s">
         <v>60</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2" t="s">
@@ -1463,10 +1471,10 @@
         <v>41</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F39" t="s">
         <v>60</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2" t="s">
@@ -1484,10 +1492,10 @@
         <v>41</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="G40" s="2"/>
       <c r="H40" s="2" t="s">
@@ -1504,7 +1512,7 @@
       <c r="D41" s="22"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G41" s="2"/>
       <c r="H41" s="2" t="s">
@@ -1513,7 +1521,7 @@
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>19</v>
@@ -1526,7 +1534,7 @@
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>19</v>
@@ -1543,7 +1551,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B44" s="14" t="s">
         <v>43</v>
       </c>
@@ -1554,14 +1562,14 @@
         <v>41</v>
       </c>
       <c r="E44" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6">
-        <v>0</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="F44" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="G44" s="6"/>
       <c r="H44" s="8" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
@@ -1569,12 +1577,12 @@
         <v>13</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D45" s="22"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G45" s="2">
         <v>0</v>
@@ -1584,19 +1592,19 @@
       </c>
     </row>
     <row r="46" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B46" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="C46" s="31"/>
-      <c r="D46" s="31"/>
-      <c r="E46" s="31"/>
-      <c r="F46" s="31"/>
-      <c r="G46" s="31"/>
-      <c r="H46" s="31"/>
+      <c r="B46" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="C46" s="37"/>
+      <c r="D46" s="37"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="37"/>
+      <c r="G46" s="37"/>
+      <c r="H46" s="37"/>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" s="25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C47" s="26"/>
       <c r="D47" s="27"/>
@@ -1607,7 +1615,7 @@
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B48" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C48" s="26"/>
       <c r="D48" s="27"/>
@@ -1618,7 +1626,7 @@
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" s="25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C49" s="26"/>
       <c r="D49" s="27"/>
@@ -1629,7 +1637,7 @@
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C50" s="26"/>
       <c r="D50" s="27"/>
@@ -1640,7 +1648,7 @@
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C51" s="26"/>
       <c r="D51" s="27"/>
@@ -1651,7 +1659,7 @@
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C52" s="26"/>
       <c r="D52" s="27"/>
@@ -1662,7 +1670,7 @@
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B53" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C53" s="26"/>
       <c r="D53" s="27"/>
@@ -1673,7 +1681,7 @@
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C54" s="26"/>
       <c r="D54" s="27"/>
@@ -1684,7 +1692,7 @@
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B55" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C55" s="26"/>
       <c r="D55" s="27"/>
@@ -1695,7 +1703,7 @@
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56" s="28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C56" s="10"/>
       <c r="D56" s="29"/>
@@ -1705,19 +1713,19 @@
       <c r="H56" s="10"/>
     </row>
     <row r="57" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B57" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="C57" s="31"/>
-      <c r="D57" s="31"/>
-      <c r="E57" s="31"/>
-      <c r="F57" s="31"/>
-      <c r="G57" s="31"/>
-      <c r="H57" s="31"/>
+      <c r="B57" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="C57" s="37"/>
+      <c r="D57" s="37"/>
+      <c r="E57" s="37"/>
+      <c r="F57" s="37"/>
+      <c r="G57" s="37"/>
+      <c r="H57" s="37"/>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B58" s="30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C58" s="10"/>
       <c r="D58" s="29"/>
@@ -1728,7 +1736,7 @@
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B59" s="30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C59" s="10"/>
       <c r="D59" s="29"/>

</xml_diff>